<commit_message>
Run 5 6 update
Added behavior for run 5 6
Updated Date in expKey and fixed date variable type throughout
Fixed wrong session for all new files
updated master table
fixed checkSessiodates
</commit_message>
<xml_diff>
--- a/Golden R01 Behavior Master Key.xlsx
+++ b/Golden R01 Behavior Master Key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Todd Appleby\Documents\Fent\CoffeyBehavior\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DrCoffey\Documents\GitHub\CoffeyBehavior\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0941EA-5B03-49CB-896D-B9C4ACAAEAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A425E4-9E37-4721-B8C4-3021CA5A3601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="75">
   <si>
     <t>TagNumber</t>
   </si>
@@ -329,13 +329,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,8 +355,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{53C3D0ED-7493-433A-A73D-0447F5E34631}" name="Table1" displayName="Table1" ref="A1:X105" totalsRowShown="0">
-  <autoFilter ref="A1:X105" xr:uid="{53C3D0ED-7493-433A-A73D-0447F5E34631}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{53C3D0ED-7493-433A-A73D-0447F5E34631}" name="Table1" displayName="Table1" ref="A1:X128" totalsRowShown="0">
+  <autoFilter ref="A1:X128" xr:uid="{53C3D0ED-7493-433A-A73D-0447F5E34631}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X36">
     <sortCondition descending="1" ref="J1:J49"/>
   </sortState>
@@ -652,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X105"/>
+  <dimension ref="A1:X128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C71" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q102" sqref="Q102"/>
+    <sheetView tabSelected="1" topLeftCell="K94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D132" sqref="D132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6305,6 +6306,949 @@
         <v>73</v>
       </c>
     </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>73</v>
+      </c>
+      <c r="B106">
+        <v>105</v>
+      </c>
+      <c r="C106">
+        <v>6</v>
+      </c>
+      <c r="E106" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F106" t="s">
+        <v>23</v>
+      </c>
+      <c r="G106" t="s">
+        <v>24</v>
+      </c>
+      <c r="I106">
+        <v>9</v>
+      </c>
+      <c r="J106" t="s">
+        <v>26</v>
+      </c>
+      <c r="K106" t="b">
+        <v>1</v>
+      </c>
+      <c r="L106" t="b">
+        <v>1</v>
+      </c>
+      <c r="M106" t="b">
+        <v>1</v>
+      </c>
+      <c r="N106" t="b">
+        <v>0</v>
+      </c>
+      <c r="O106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>74</v>
+      </c>
+      <c r="B107">
+        <v>106</v>
+      </c>
+      <c r="C107">
+        <v>6</v>
+      </c>
+      <c r="E107" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F107" t="s">
+        <v>23</v>
+      </c>
+      <c r="G107" t="s">
+        <v>24</v>
+      </c>
+      <c r="I107">
+        <v>10</v>
+      </c>
+      <c r="J107" t="s">
+        <v>26</v>
+      </c>
+      <c r="K107" t="b">
+        <v>1</v>
+      </c>
+      <c r="L107" t="b">
+        <v>1</v>
+      </c>
+      <c r="M107" t="b">
+        <v>1</v>
+      </c>
+      <c r="N107" t="b">
+        <v>0</v>
+      </c>
+      <c r="O107" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>75</v>
+      </c>
+      <c r="B108">
+        <v>107</v>
+      </c>
+      <c r="C108">
+        <v>6</v>
+      </c>
+      <c r="E108" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F108" t="s">
+        <v>23</v>
+      </c>
+      <c r="G108" t="s">
+        <v>24</v>
+      </c>
+      <c r="I108">
+        <v>11</v>
+      </c>
+      <c r="J108" t="s">
+        <v>26</v>
+      </c>
+      <c r="K108" t="b">
+        <v>1</v>
+      </c>
+      <c r="L108" t="b">
+        <v>1</v>
+      </c>
+      <c r="M108" t="b">
+        <v>1</v>
+      </c>
+      <c r="N108" t="b">
+        <v>0</v>
+      </c>
+      <c r="O108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>76</v>
+      </c>
+      <c r="B109">
+        <v>108</v>
+      </c>
+      <c r="C109">
+        <v>6</v>
+      </c>
+      <c r="E109" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F109" t="s">
+        <v>23</v>
+      </c>
+      <c r="G109" t="s">
+        <v>24</v>
+      </c>
+      <c r="I109">
+        <v>12</v>
+      </c>
+      <c r="J109" t="s">
+        <v>26</v>
+      </c>
+      <c r="K109" t="b">
+        <v>1</v>
+      </c>
+      <c r="L109" t="b">
+        <v>1</v>
+      </c>
+      <c r="M109" t="b">
+        <v>1</v>
+      </c>
+      <c r="N109" t="b">
+        <v>0</v>
+      </c>
+      <c r="O109" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>77</v>
+      </c>
+      <c r="B110">
+        <v>109</v>
+      </c>
+      <c r="C110">
+        <v>6</v>
+      </c>
+      <c r="E110" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F110" t="s">
+        <v>23</v>
+      </c>
+      <c r="G110" t="s">
+        <v>24</v>
+      </c>
+      <c r="I110">
+        <v>13</v>
+      </c>
+      <c r="J110" t="s">
+        <v>26</v>
+      </c>
+      <c r="K110" t="b">
+        <v>1</v>
+      </c>
+      <c r="L110" t="b">
+        <v>1</v>
+      </c>
+      <c r="M110" t="b">
+        <v>1</v>
+      </c>
+      <c r="N110" t="b">
+        <v>0</v>
+      </c>
+      <c r="O110" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>78</v>
+      </c>
+      <c r="B111">
+        <v>110</v>
+      </c>
+      <c r="C111">
+        <v>6</v>
+      </c>
+      <c r="E111" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F111" t="s">
+        <v>23</v>
+      </c>
+      <c r="G111" t="s">
+        <v>24</v>
+      </c>
+      <c r="I111">
+        <v>14</v>
+      </c>
+      <c r="J111" t="s">
+        <v>26</v>
+      </c>
+      <c r="K111" t="b">
+        <v>1</v>
+      </c>
+      <c r="L111" t="b">
+        <v>1</v>
+      </c>
+      <c r="M111" t="b">
+        <v>1</v>
+      </c>
+      <c r="N111" t="b">
+        <v>0</v>
+      </c>
+      <c r="O111" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>79</v>
+      </c>
+      <c r="B112">
+        <v>111</v>
+      </c>
+      <c r="C112">
+        <v>6</v>
+      </c>
+      <c r="E112" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F112" t="s">
+        <v>32</v>
+      </c>
+      <c r="G112" t="s">
+        <v>24</v>
+      </c>
+      <c r="I112">
+        <v>15</v>
+      </c>
+      <c r="J112" t="s">
+        <v>26</v>
+      </c>
+      <c r="K112" t="b">
+        <v>1</v>
+      </c>
+      <c r="L112" t="b">
+        <v>1</v>
+      </c>
+      <c r="M112" t="b">
+        <v>1</v>
+      </c>
+      <c r="N112" t="b">
+        <v>0</v>
+      </c>
+      <c r="O112" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>80</v>
+      </c>
+      <c r="B113">
+        <v>112</v>
+      </c>
+      <c r="C113">
+        <v>6</v>
+      </c>
+      <c r="E113" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F113" t="s">
+        <v>32</v>
+      </c>
+      <c r="G113" t="s">
+        <v>24</v>
+      </c>
+      <c r="I113">
+        <v>16</v>
+      </c>
+      <c r="J113" t="s">
+        <v>26</v>
+      </c>
+      <c r="K113" t="b">
+        <v>1</v>
+      </c>
+      <c r="L113" t="b">
+        <v>1</v>
+      </c>
+      <c r="M113" t="b">
+        <v>1</v>
+      </c>
+      <c r="N113" t="b">
+        <v>0</v>
+      </c>
+      <c r="O113" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>81</v>
+      </c>
+      <c r="B114">
+        <v>113</v>
+      </c>
+      <c r="C114">
+        <v>6</v>
+      </c>
+      <c r="E114" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F114" t="s">
+        <v>32</v>
+      </c>
+      <c r="G114" t="s">
+        <v>24</v>
+      </c>
+      <c r="I114">
+        <v>17</v>
+      </c>
+      <c r="J114" t="s">
+        <v>26</v>
+      </c>
+      <c r="K114" t="b">
+        <v>1</v>
+      </c>
+      <c r="L114" t="b">
+        <v>1</v>
+      </c>
+      <c r="M114" t="b">
+        <v>1</v>
+      </c>
+      <c r="N114" t="b">
+        <v>0</v>
+      </c>
+      <c r="O114" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>82</v>
+      </c>
+      <c r="B115">
+        <v>114</v>
+      </c>
+      <c r="C115">
+        <v>6</v>
+      </c>
+      <c r="E115" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F115" t="s">
+        <v>32</v>
+      </c>
+      <c r="G115" t="s">
+        <v>24</v>
+      </c>
+      <c r="I115">
+        <v>18</v>
+      </c>
+      <c r="J115" t="s">
+        <v>26</v>
+      </c>
+      <c r="K115" t="b">
+        <v>1</v>
+      </c>
+      <c r="L115" t="b">
+        <v>1</v>
+      </c>
+      <c r="M115" t="b">
+        <v>1</v>
+      </c>
+      <c r="N115" t="b">
+        <v>0</v>
+      </c>
+      <c r="O115" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>83</v>
+      </c>
+      <c r="B116">
+        <v>115</v>
+      </c>
+      <c r="C116">
+        <v>6</v>
+      </c>
+      <c r="E116" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F116" t="s">
+        <v>32</v>
+      </c>
+      <c r="G116" t="s">
+        <v>24</v>
+      </c>
+      <c r="I116">
+        <v>19</v>
+      </c>
+      <c r="J116" t="s">
+        <v>26</v>
+      </c>
+      <c r="K116" t="b">
+        <v>1</v>
+      </c>
+      <c r="L116" t="b">
+        <v>1</v>
+      </c>
+      <c r="M116" t="b">
+        <v>1</v>
+      </c>
+      <c r="N116" t="b">
+        <v>0</v>
+      </c>
+      <c r="O116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>84</v>
+      </c>
+      <c r="B117">
+        <v>116</v>
+      </c>
+      <c r="C117">
+        <v>6</v>
+      </c>
+      <c r="E117" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F117" t="s">
+        <v>32</v>
+      </c>
+      <c r="G117" t="s">
+        <v>24</v>
+      </c>
+      <c r="I117">
+        <v>20</v>
+      </c>
+      <c r="J117" t="s">
+        <v>44</v>
+      </c>
+      <c r="K117" t="b">
+        <v>1</v>
+      </c>
+      <c r="L117" t="b">
+        <v>1</v>
+      </c>
+      <c r="M117" t="b">
+        <v>1</v>
+      </c>
+      <c r="N117" t="b">
+        <v>0</v>
+      </c>
+      <c r="O117" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>85</v>
+      </c>
+      <c r="B118">
+        <v>117</v>
+      </c>
+      <c r="C118">
+        <v>6</v>
+      </c>
+      <c r="E118" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F118" t="s">
+        <v>23</v>
+      </c>
+      <c r="G118" t="s">
+        <v>24</v>
+      </c>
+      <c r="I118">
+        <v>9</v>
+      </c>
+      <c r="J118" t="s">
+        <v>44</v>
+      </c>
+      <c r="K118" t="b">
+        <v>1</v>
+      </c>
+      <c r="L118" t="b">
+        <v>1</v>
+      </c>
+      <c r="M118" t="b">
+        <v>1</v>
+      </c>
+      <c r="N118" t="b">
+        <v>0</v>
+      </c>
+      <c r="O118" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>86</v>
+      </c>
+      <c r="B119">
+        <v>118</v>
+      </c>
+      <c r="C119">
+        <v>6</v>
+      </c>
+      <c r="E119" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F119" t="s">
+        <v>23</v>
+      </c>
+      <c r="G119" t="s">
+        <v>24</v>
+      </c>
+      <c r="I119">
+        <v>10</v>
+      </c>
+      <c r="J119" t="s">
+        <v>44</v>
+      </c>
+      <c r="K119" t="b">
+        <v>1</v>
+      </c>
+      <c r="L119" t="b">
+        <v>1</v>
+      </c>
+      <c r="M119" t="b">
+        <v>1</v>
+      </c>
+      <c r="N119" t="b">
+        <v>0</v>
+      </c>
+      <c r="O119" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>87</v>
+      </c>
+      <c r="B120">
+        <v>119</v>
+      </c>
+      <c r="C120">
+        <v>6</v>
+      </c>
+      <c r="E120" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F120" t="s">
+        <v>23</v>
+      </c>
+      <c r="G120" t="s">
+        <v>24</v>
+      </c>
+      <c r="I120">
+        <v>11</v>
+      </c>
+      <c r="J120" t="s">
+        <v>44</v>
+      </c>
+      <c r="K120" t="b">
+        <v>1</v>
+      </c>
+      <c r="L120" t="b">
+        <v>1</v>
+      </c>
+      <c r="M120" t="b">
+        <v>1</v>
+      </c>
+      <c r="N120" t="b">
+        <v>0</v>
+      </c>
+      <c r="O120" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>88</v>
+      </c>
+      <c r="B121">
+        <v>120</v>
+      </c>
+      <c r="C121">
+        <v>6</v>
+      </c>
+      <c r="E121" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F121" t="s">
+        <v>23</v>
+      </c>
+      <c r="G121" t="s">
+        <v>24</v>
+      </c>
+      <c r="I121">
+        <v>12</v>
+      </c>
+      <c r="J121" t="s">
+        <v>44</v>
+      </c>
+      <c r="K121" t="b">
+        <v>1</v>
+      </c>
+      <c r="L121" t="b">
+        <v>1</v>
+      </c>
+      <c r="M121" t="b">
+        <v>1</v>
+      </c>
+      <c r="N121" t="b">
+        <v>0</v>
+      </c>
+      <c r="O121" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>89</v>
+      </c>
+      <c r="B122">
+        <v>121</v>
+      </c>
+      <c r="C122">
+        <v>6</v>
+      </c>
+      <c r="E122" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F122" t="s">
+        <v>23</v>
+      </c>
+      <c r="G122" t="s">
+        <v>24</v>
+      </c>
+      <c r="I122">
+        <v>13</v>
+      </c>
+      <c r="J122" t="s">
+        <v>44</v>
+      </c>
+      <c r="K122" t="b">
+        <v>1</v>
+      </c>
+      <c r="L122" t="b">
+        <v>1</v>
+      </c>
+      <c r="M122" t="b">
+        <v>1</v>
+      </c>
+      <c r="N122" t="b">
+        <v>0</v>
+      </c>
+      <c r="O122" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>90</v>
+      </c>
+      <c r="B123">
+        <v>122</v>
+      </c>
+      <c r="C123">
+        <v>6</v>
+      </c>
+      <c r="E123" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F123" t="s">
+        <v>32</v>
+      </c>
+      <c r="G123" t="s">
+        <v>24</v>
+      </c>
+      <c r="I123">
+        <v>15</v>
+      </c>
+      <c r="J123" t="s">
+        <v>44</v>
+      </c>
+      <c r="K123" t="b">
+        <v>1</v>
+      </c>
+      <c r="L123" t="b">
+        <v>1</v>
+      </c>
+      <c r="M123" t="b">
+        <v>1</v>
+      </c>
+      <c r="N123" t="b">
+        <v>0</v>
+      </c>
+      <c r="O123" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>91</v>
+      </c>
+      <c r="B124">
+        <v>123</v>
+      </c>
+      <c r="C124">
+        <v>6</v>
+      </c>
+      <c r="E124" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F124" t="s">
+        <v>32</v>
+      </c>
+      <c r="G124" t="s">
+        <v>24</v>
+      </c>
+      <c r="I124">
+        <v>16</v>
+      </c>
+      <c r="J124" t="s">
+        <v>44</v>
+      </c>
+      <c r="K124" t="b">
+        <v>1</v>
+      </c>
+      <c r="L124" t="b">
+        <v>1</v>
+      </c>
+      <c r="M124" t="b">
+        <v>1</v>
+      </c>
+      <c r="N124" t="b">
+        <v>0</v>
+      </c>
+      <c r="O124" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>92</v>
+      </c>
+      <c r="B125">
+        <v>124</v>
+      </c>
+      <c r="C125">
+        <v>6</v>
+      </c>
+      <c r="E125" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F125" t="s">
+        <v>32</v>
+      </c>
+      <c r="G125" t="s">
+        <v>24</v>
+      </c>
+      <c r="I125">
+        <v>17</v>
+      </c>
+      <c r="J125" t="s">
+        <v>44</v>
+      </c>
+      <c r="K125" t="b">
+        <v>1</v>
+      </c>
+      <c r="L125" t="b">
+        <v>1</v>
+      </c>
+      <c r="M125" t="b">
+        <v>1</v>
+      </c>
+      <c r="N125" t="b">
+        <v>0</v>
+      </c>
+      <c r="O125" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>93</v>
+      </c>
+      <c r="B126">
+        <v>125</v>
+      </c>
+      <c r="C126">
+        <v>6</v>
+      </c>
+      <c r="E126" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F126" t="s">
+        <v>32</v>
+      </c>
+      <c r="G126" t="s">
+        <v>24</v>
+      </c>
+      <c r="I126">
+        <v>18</v>
+      </c>
+      <c r="J126" t="s">
+        <v>44</v>
+      </c>
+      <c r="K126" t="b">
+        <v>1</v>
+      </c>
+      <c r="L126" t="b">
+        <v>1</v>
+      </c>
+      <c r="M126" t="b">
+        <v>1</v>
+      </c>
+      <c r="N126" t="b">
+        <v>0</v>
+      </c>
+      <c r="O126" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>94</v>
+      </c>
+      <c r="B127">
+        <v>126</v>
+      </c>
+      <c r="C127">
+        <v>6</v>
+      </c>
+      <c r="E127" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F127" t="s">
+        <v>32</v>
+      </c>
+      <c r="G127" t="s">
+        <v>24</v>
+      </c>
+      <c r="I127">
+        <v>19</v>
+      </c>
+      <c r="J127" t="s">
+        <v>44</v>
+      </c>
+      <c r="K127" t="b">
+        <v>1</v>
+      </c>
+      <c r="L127" t="b">
+        <v>1</v>
+      </c>
+      <c r="M127" t="b">
+        <v>1</v>
+      </c>
+      <c r="N127" t="b">
+        <v>0</v>
+      </c>
+      <c r="O127" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>95</v>
+      </c>
+      <c r="B128">
+        <v>127</v>
+      </c>
+      <c r="C128">
+        <v>6</v>
+      </c>
+      <c r="E128" s="6">
+        <v>45660</v>
+      </c>
+      <c r="F128" t="s">
+        <v>32</v>
+      </c>
+      <c r="G128" t="s">
+        <v>24</v>
+      </c>
+      <c r="I128">
+        <v>20</v>
+      </c>
+      <c r="J128" t="s">
+        <v>44</v>
+      </c>
+      <c r="K128" t="b">
+        <v>1</v>
+      </c>
+      <c r="L128" t="b">
+        <v>1</v>
+      </c>
+      <c r="M128" t="b">
+        <v>1</v>
+      </c>
+      <c r="N128" t="b">
+        <v>0</v>
+      </c>
+      <c r="O128" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>